<commit_message>
code cleanup, file organization
</commit_message>
<xml_diff>
--- a/outputs/cluster_8v_results_cleaned.xlsx
+++ b/outputs/cluster_8v_results_cleaned.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m_carper\Documents\GitHub\NYC-PUMA-Economic-Clusters\outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcarp\GitHub\NYC-Neighborhood-Clustering\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6EEAE4F-7154-4CA6-B85F-3D48AD74F9DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4148DFF4-B12B-4331-A60A-DA447556BFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>labels</t>
   </si>
@@ -87,6 +87,12 @@
   <si>
     <t>Cluster 0</t>
   </si>
+  <si>
+    <t>Indicator</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
 </sst>
 </file>
 
@@ -134,16 +140,18 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -176,37 +184,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -853,6 +831,7 @@
         <c:axId val="1813996015"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -981,7 +960,669 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cluster 0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>park_perc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>job_perc</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>comp_access</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>bach_degr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>empl_rate</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>rent_under30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>subway_sbs</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>infant_mortality_per1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>PUMA_count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$J$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>75.547368421052639</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95.257894736842104</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75.336842105263159</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.921052631578952</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44.742105263157903</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43.734147331483733</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.207292105263158</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2915-4734-96FE-C6E7A188F5D1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cluster 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>park_perc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>job_perc</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>comp_access</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>bach_degr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>empl_rate</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>rent_under30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>subway_sbs</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>infant_mortality_per1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>PUMA_count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$J$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>96.978571428571428</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98.914285714285711</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66.26428571428572</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.06428571428571</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90.814285714285717</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42.971428571428582</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>67.994487045183334</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.7172971428571424</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2915-4734-96FE-C6E7A188F5D1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cluster 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>park_perc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>job_perc</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>comp_access</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>bach_degr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>empl_rate</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>rent_under30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>subway_sbs</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>infant_mortality_per1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>PUMA_count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$4:$J$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>67.493333333333325</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.493333333333332</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>76.72</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27.926666666666669</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>93.513333333333335</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>46.02</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22.260182862146959</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.8105460000000004</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2915-4734-96FE-C6E7A188F5D1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Cluster 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>park_perc</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>job_perc</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>comp_access</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>bach_degr</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>empl_rate</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>rent_under30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>subway_sbs</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>infant_mortality_per1000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>PUMA_count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>95.414285714285711</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>89.614285714285714</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76.857142857142861</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>95.814285714285717</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.51428571428572</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>72.368109708664079</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7423714285714289</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2915-4734-96FE-C6E7A188F5D1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="423835472"/>
+        <c:axId val="423837584"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="423835472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="423837584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="423837584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="423835472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1524,20 +2165,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147636</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1047750</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1557,6 +2701,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8023AD34-D2A5-0A35-1CBF-C1D8217A75EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1853,20 +3033,22 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I5"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="74.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1894,7 +3076,7 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -1902,194 +3084,202 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>75.547368421052639</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>95.257894736842104</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>75.336842105263159</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>35.921052631578952</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>94</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>44.742105263157903</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>43.734147331483733</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>3.207292105263158</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>96.978571428571428</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>98.914285714285711</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>66.26428571428572</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>28.06428571428571</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>90.814285714285717</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>42.971428571428582</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>67.994487045183334</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>4.7172971428571424</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>67.493333333333325</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>39.493333333333332</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>76.72</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>27.926666666666669</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>93.513333333333335</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>46.02</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>22.260182862146959</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>4.8105460000000004</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>95.414285714285711</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>100</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>89.614285714285714</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>76.857142857142861</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>95.814285714285717</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>60.51428571428572</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>72.368109708664079</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>1.7423714285714289</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5">
         <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C10" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C11" t="s">
+      <c r="B11" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C13" t="s">
+      <c r="B13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C15" t="s">
+      <c r="B15" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>